<commit_message>
03/24/23: Leetcode & Python Internal
</commit_message>
<xml_diff>
--- a/Algorithms/Leetcode/Leetcode Catalog - Yu Wang.xlsx
+++ b/Algorithms/Leetcode/Leetcode Catalog - Yu Wang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuwang/Desktop/Notes/Algorithms/Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C812B44A-5DD6-C943-AEDD-4FF686AFDC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D824F3B-A021-394E-8B07-350F96CEE9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="500" windowWidth="28040" windowHeight="15920" firstSheet="9" activeTab="21" xr2:uid="{D74CB876-27C2-064D-BD73-4428B59FF732}"/>
+    <workbookView xWindow="300" yWindow="500" windowWidth="28040" windowHeight="15920" firstSheet="9" activeTab="15" xr2:uid="{D74CB876-27C2-064D-BD73-4428B59FF732}"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="5" r:id="rId1"/>
@@ -28,15 +28,14 @@
     <sheet name="Greedy" sheetId="13" r:id="rId13"/>
     <sheet name="Sheet2" sheetId="25" r:id="rId14"/>
     <sheet name="Two Pointers" sheetId="14" r:id="rId15"/>
-    <sheet name="Sheet1" sheetId="24" r:id="rId16"/>
-    <sheet name="Graph" sheetId="15" r:id="rId17"/>
-    <sheet name="Backtrack" sheetId="16" r:id="rId18"/>
-    <sheet name="Math" sheetId="17" r:id="rId19"/>
-    <sheet name="Bit" sheetId="18" r:id="rId20"/>
-    <sheet name="Sliding Window" sheetId="19" r:id="rId21"/>
-    <sheet name="Simulation" sheetId="20" r:id="rId22"/>
-    <sheet name="OOD" sheetId="21" r:id="rId23"/>
-    <sheet name="Combined" sheetId="23" r:id="rId24"/>
+    <sheet name="Graph" sheetId="15" r:id="rId16"/>
+    <sheet name="Backtrack" sheetId="16" r:id="rId17"/>
+    <sheet name="Math" sheetId="17" r:id="rId18"/>
+    <sheet name="Bit" sheetId="18" r:id="rId19"/>
+    <sheet name="Sliding Window" sheetId="19" r:id="rId20"/>
+    <sheet name="Simulation" sheetId="20" r:id="rId21"/>
+    <sheet name="OOD" sheetId="21" r:id="rId22"/>
+    <sheet name="Combined" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="350">
   <si>
     <t>#</t>
   </si>
@@ -1101,13 +1100,19 @@
   </si>
   <si>
     <t>2221 数组的三角和</t>
+  </si>
+  <si>
+    <t>818 赛车</t>
+  </si>
+  <si>
+    <t>1293 网格中的最短路径</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1235,6 +1240,21 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="20"/>
+      <color theme="10"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1257,7 +1277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1275,7 +1295,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1303,10 +1322,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1630,325 +1656,325 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="58.83203125" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="58.83203125" style="15"/>
+    <col min="1" max="16384" width="58.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
+      <c r="A2" s="15">
         <v>283</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>566</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>485</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="16" t="s">
+      <c r="B4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <v>645</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>697</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="16">
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15">
         <v>20220918</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="16">
+      <c r="B8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15">
         <v>20220917</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>240</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>378</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="B10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>287</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="16" t="s">
+      <c r="B11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>667</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
+      <c r="A13" s="15">
         <v>565</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="16" t="s">
+      <c r="B13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="16">
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15">
         <v>20220919</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="16">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="16">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15">
         <v>20220620</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="16">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15">
         <v>20220625</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="16">
+      <c r="B18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15">
         <v>20220822</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="16">
+      <c r="B19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="15">
         <v>20220822</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="16">
+      <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15">
         <v>20220822</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="16">
+      <c r="B21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15">
         <v>20220922</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="16">
+      <c r="B22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="15">
         <v>20221213</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="16">
+      <c r="B23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="15">
         <v>20230315</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="16">
+      <c r="B24" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="15">
         <v>20221229</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="16">
+      <c r="B25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="15">
         <v>20221230</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="16">
+      <c r="B26" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="15">
         <v>20221231</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="16">
+      <c r="B27" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="15">
         <v>20221231</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="15">
         <v>20211229</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="16">
+      <c r="B29" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="15">
         <v>20230323</v>
       </c>
     </row>
@@ -2361,612 +2387,623 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF52CBDF-A54F-B64B-ABC7-BC9DA66EFACF}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C54" sqref="A54:C54"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="19" style="11" customWidth="1"/>
-    <col min="3" max="3" width="29.5" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="11"/>
+    <col min="1" max="1" width="53.6640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="19" style="22" customWidth="1"/>
+    <col min="3" max="3" width="29.5" style="22" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
         <v>70</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
         <v>303</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15">
         <v>20220829</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15">
         <v>20220829</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15">
         <v>20220829</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15">
         <v>20220828</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
         <v>62</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
         <v>413</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
         <v>343</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="B10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
         <v>279</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="B11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15">
         <v>20220826</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="15">
         <v>646</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
         <v>376</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
         <v>1143</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15">
         <v>20220827</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15">
         <v>20220828</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
         <v>474</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="B19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15">
         <v>20220825</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15">
         <v>20220827</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
         <v>139</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="B22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="B23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="15">
         <v>20220827</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
         <v>309</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="B24" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="15">
         <v>20221226</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B26" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="15">
         <v>20220925</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2">
+      <c r="B27" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="15">
         <v>20220610</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B28" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="15">
         <v>20220710</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B29" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="15">
         <v>20220827</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="B30" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="15">
         <v>20220827</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2">
+      <c r="B31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="15">
         <v>20220827</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="2">
+      <c r="B32" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="15">
         <v>20220828</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2">
+      <c r="B33" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="15">
         <v>20220829</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="2">
+      <c r="B34" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="15">
         <v>20220831</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2">
+      <c r="B35" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="15">
         <v>20220831</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2">
+      <c r="B36" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="15">
         <v>20220831</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2">
+      <c r="B37" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="15">
         <v>20220912</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="2">
+      <c r="B38" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="15">
         <v>20220923</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="2">
+      <c r="B39" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="15">
         <v>20220925</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2">
+      <c r="B40" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="15">
         <v>20230308</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="15">
         <v>20221129</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="15">
         <v>20220827</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="15">
         <v>20220827</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="15">
         <v>20220827</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="15">
         <v>20220828</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="15">
         <v>20220828</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="15">
         <v>20220828</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="15">
         <v>20220828</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="15">
         <v>20220831</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="15">
         <v>20220831</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="15">
         <v>20230103</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="15">
         <v>20230313</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="15">
         <v>20230314</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="23" t="s">
         <v>341</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="15">
         <v>20230322</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="18">
+        <v>20230324</v>
       </c>
     </row>
   </sheetData>
@@ -3015,6 +3052,7 @@
     <hyperlink ref="A52" r:id="rId39" display="https://leetcode.cn/problems/substring-with-largest-variance/solution/2272-zui-da-bo-dong-de-zi-zi-fu-chuan-dp-zai2/" xr:uid="{C4E39D24-CA1B-4D4F-84FE-5A9F21DBFEF2}"/>
     <hyperlink ref="A53" r:id="rId40" display="https://leetcode.cn/problems/maximum-number-of-books-you-can-take/solution/2355-ni-neng-na-zou-de-zui-da-tu-shu-shu-4cwe/" xr:uid="{CFA00C0F-A1B9-2143-9567-C1D46DE839B4}"/>
     <hyperlink ref="A54" r:id="rId41" xr:uid="{143774B1-1CB5-584A-A7EA-EFB7FAE785C2}"/>
+    <hyperlink ref="A55" r:id="rId42" xr:uid="{9CE5EBF7-DFF5-8C4C-800C-035221F3521C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3030,383 +3068,383 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="67.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="11"/>
-    <col min="3" max="3" width="22.83203125" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="11"/>
+    <col min="1" max="1" width="67.6640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="10"/>
+    <col min="3" max="3" width="22.83203125" style="10" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
+      <c r="A2" s="15">
         <v>455</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>121</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>122</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="16" t="s">
+      <c r="B4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <v>605</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>392</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>665</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="16">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15">
         <v>20220829</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="16">
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15">
         <v>20220829</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>406</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="B10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="16">
+      <c r="B11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15">
         <v>20230317</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>763</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="16">
+      <c r="B13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15">
         <v>20230312</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="16">
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15">
         <v>20230312</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="16">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15">
         <v>20220911</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="16">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15">
         <v>20221129</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="16">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15">
         <v>20220727</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="16">
+      <c r="B18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15">
         <v>20220911</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="16">
+      <c r="B19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="15">
         <v>20220924</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="16">
+      <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15">
         <v>20221011</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="16">
+      <c r="B21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15">
         <v>20230311</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="16">
+      <c r="B22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="15">
         <v>20230318</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="16">
+      <c r="B23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="15">
         <v>20221017</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="16">
+      <c r="B24" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="15">
         <v>20221017</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="16">
+      <c r="B25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="15">
         <v>20221019</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="16">
+      <c r="B26" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="15">
         <v>20221207</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="16">
+      <c r="B27" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="15">
         <v>20230307</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="16">
+      <c r="B28" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="15">
         <v>20230307</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="16">
+      <c r="B29" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="15">
         <v>20230311</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="15">
         <v>20220913</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="16">
+      <c r="C31" s="15">
         <v>20220919</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="16">
+      <c r="B32" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="15">
         <v>20230321</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="15">
         <v>20230322</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="17" t="s">
         <v>346</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="16">
+      <c r="B34" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="15">
         <v>20230323</v>
       </c>
     </row>
@@ -3467,288 +3505,288 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.83203125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="19"/>
-    <col min="3" max="3" width="14.83203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="19"/>
+    <col min="1" max="1" width="42.83203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="18"/>
+    <col min="3" max="3" width="14.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
+      <c r="A2" s="15">
         <v>167</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16"/>
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>633</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="16"/>
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>345</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="16"/>
+      <c r="B4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <v>680</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="16"/>
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>88</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="16"/>
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>141</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="16"/>
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="16" t="s">
+      <c r="B8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="16">
+      <c r="B9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="15">
         <v>20220610</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="16">
+      <c r="B10" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="15">
         <v>20220615</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="16">
+      <c r="B11" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="15">
         <v>20221221</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>524</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="16"/>
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="16">
+      <c r="B13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15">
         <v>20220926</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="16">
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15">
         <v>20220905</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="16">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15">
         <v>20211225</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="16">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15">
         <v>20220913</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="16">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15">
         <v>20220625</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="16">
+      <c r="B18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15">
         <v>20220918</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="16">
+      <c r="B19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="15">
         <v>20220919</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="16">
+      <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15">
         <v>20221221</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="16">
+      <c r="B21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15">
         <v>20221221</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="16">
+      <c r="B22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="15">
         <v>20221222</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="16">
+      <c r="B23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="15">
         <v>20221229</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="15">
         <v>20211229</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="15">
         <v>20220905</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="19">
+      <c r="B27" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="18">
         <v>20230323</v>
       </c>
     </row>
@@ -3782,399 +3820,391 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFC598EB-09F3-404C-9B2A-92FB7D1755E3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3390D82-F280-2841-A652-0961C2865E3C}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="4"/>
-    <col min="3" max="3" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="15">
+        <v>20220912</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="15">
+        <v>20220920</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15">
+        <v>20230217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15">
+        <v>20230216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15">
+        <v>20230216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15">
+        <v>20230217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15">
+        <v>20230312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
+    </row>
+    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15">
+        <v>20220612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15">
         <v>20220912</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>20220920</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>20230217</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>20230216</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>20230216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>20230217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2">
-        <v>20230312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2">
-        <v>20220612</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2">
-        <v>20220912</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15">
         <v>20220914</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15">
         <v>20220917</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15">
         <v>20220926</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15">
         <v>20221020</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="19" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="15">
         <v>20230220</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="20" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C20" s="15">
         <v>20221018</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="21" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="15">
+        <v>20230324</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="15">
         <v>20230220</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+    </row>
+    <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="B24" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="15">
         <v>20220925</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="15">
         <v>20230219</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B26" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="15">
         <v>20220906</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2">
+      <c r="B27" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="15">
         <v>20220906</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B28" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="15">
         <v>20220906</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B29" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="15">
         <v>20220906</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="B30" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="15">
         <v>20220906</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2">
+      <c r="B31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="15">
         <v>20220906</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="15">
         <v>20220913</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="15">
         <v>20220923</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="15">
         <v>20230308</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="15">
         <v>20230319</v>
       </c>
     </row>
@@ -4189,8 +4219,8 @@
       <c r="C37" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:C22">
-    <sortCondition ref="B12:B22" customList="E,M,H"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:C22">
+    <sortCondition ref="B11:B22" customList="E,M,H"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://leetcode.cn/problems/all-paths-from-source-to-target/solution/by-wywy-m-nqp0/" xr:uid="{62AA1BDA-9AEF-1D4E-985F-E4BFC300F9ED}"/>
@@ -4200,16 +4230,16 @@
     <hyperlink ref="A7" r:id="rId5" display="https://leetcode.cn/problems/course-schedule-ii/solution/210-ke-cheng-biao-iigraph-by-wywy-m-18nk/" xr:uid="{C7EEFC8F-2387-F14A-B36C-A22ACD69ECCB}"/>
     <hyperlink ref="A8" r:id="rId6" display="https://leetcode.cn/problems/network-delay-time/solution/743-wang-luo-yan-chi-shi-jian-dijkstra-b-6zyo/" xr:uid="{FC2F7E70-70B6-EC40-83E9-F14EEDE1A2B2}"/>
     <hyperlink ref="A9" r:id="rId7" display="https://leetcode.cn/problems/min-cost-to-connect-all-points/solution/1584-lian-jie-suo-you-dian-de-zui-xiao-f-dtmy/" xr:uid="{D6E252E8-6A56-B449-917D-D9191B43E8F1}"/>
-    <hyperlink ref="A12" r:id="rId8" display="https://leetcode-cn.com/problems/shortest-path-in-binary-matrix/solution/1091-er-jin-zhi-ju-zhen-zui-duan-lu-jing-00dr/" xr:uid="{678CC0D2-5BB2-9447-A9D9-85A1922DAD7A}"/>
-    <hyperlink ref="A14" r:id="rId9" display="https://leetcode.cn/problems/ji-qi-ren-de-yun-dong-fan-wei-lcof/solution/-by-wywy-m-hks2/" xr:uid="{433B27C5-3ADF-6344-8B10-3C6FE890D909}"/>
-    <hyperlink ref="A15" r:id="rId10" display="https://leetcode.cn/problems/web-crawler/solution/by-wywy-m-tq5x/" xr:uid="{1096138D-EBE2-324D-A769-E0CF4843CC45}"/>
-    <hyperlink ref="A16" r:id="rId11" display="https://leetcode.cn/problems/populating-next-right-pointers-in-each-node-ii/solution/117-by-wywy-m-2dey/" xr:uid="{DB4092D2-CEB5-5F40-9A2F-A3D1F3E1FAD5}"/>
-    <hyperlink ref="A17" r:id="rId12" display="https://leetcode.cn/problems/evaluate-division/solution/by-wywy-m-fqcc/" xr:uid="{3BA99F54-D69C-BE40-BD52-19CC44580857}"/>
-    <hyperlink ref="A18" r:id="rId13" display="https://leetcode.cn/problems/walls-and-gates/solution/286-by-wywy-m-v89r/" xr:uid="{A1807D7E-F45A-BC4D-A674-450FE3CC3465}"/>
-    <hyperlink ref="A21" r:id="rId14" display="https://leetcode.cn/problems/shortest-distance-from-all-buildings/solution/317-by-wywy-m-31q4/" xr:uid="{7C3F06B2-F6CE-D941-A3E6-9CC13D48726B}"/>
-    <hyperlink ref="A19" r:id="rId15" display="https://leetcode.cn/problems/01-matrix/solution/-by-wywy-m-1ak4/" xr:uid="{AC1F76FF-A2DA-694F-A769-2136BC16C971}"/>
+    <hyperlink ref="A11" r:id="rId8" display="https://leetcode-cn.com/problems/shortest-path-in-binary-matrix/solution/1091-er-jin-zhi-ju-zhen-zui-duan-lu-jing-00dr/" xr:uid="{678CC0D2-5BB2-9447-A9D9-85A1922DAD7A}"/>
+    <hyperlink ref="A13" r:id="rId9" display="https://leetcode.cn/problems/ji-qi-ren-de-yun-dong-fan-wei-lcof/solution/-by-wywy-m-hks2/" xr:uid="{433B27C5-3ADF-6344-8B10-3C6FE890D909}"/>
+    <hyperlink ref="A14" r:id="rId10" display="https://leetcode.cn/problems/web-crawler/solution/by-wywy-m-tq5x/" xr:uid="{1096138D-EBE2-324D-A769-E0CF4843CC45}"/>
+    <hyperlink ref="A15" r:id="rId11" display="https://leetcode.cn/problems/populating-next-right-pointers-in-each-node-ii/solution/117-by-wywy-m-2dey/" xr:uid="{DB4092D2-CEB5-5F40-9A2F-A3D1F3E1FAD5}"/>
+    <hyperlink ref="A16" r:id="rId12" display="https://leetcode.cn/problems/evaluate-division/solution/by-wywy-m-fqcc/" xr:uid="{3BA99F54-D69C-BE40-BD52-19CC44580857}"/>
+    <hyperlink ref="A17" r:id="rId13" display="https://leetcode.cn/problems/walls-and-gates/solution/286-by-wywy-m-v89r/" xr:uid="{A1807D7E-F45A-BC4D-A674-450FE3CC3465}"/>
+    <hyperlink ref="A20" r:id="rId14" display="https://leetcode.cn/problems/shortest-distance-from-all-buildings/solution/317-by-wywy-m-31q4/" xr:uid="{7C3F06B2-F6CE-D941-A3E6-9CC13D48726B}"/>
+    <hyperlink ref="A18" r:id="rId15" display="https://leetcode.cn/problems/01-matrix/solution/-by-wywy-m-1ak4/" xr:uid="{AC1F76FF-A2DA-694F-A769-2136BC16C971}"/>
     <hyperlink ref="A22" r:id="rId16" display="https://leetcode.cn/problems/sliding-puzzle/solution/773-hua-dong-mi-ti-bfs-by-ywrx-c74s/" xr:uid="{0AD32694-5038-3D45-918C-C400FC7946DE}"/>
-    <hyperlink ref="A20" r:id="rId17" display="https://leetcode.cn/problems/open-the-lock/solution/752-da-kai-zhuan-pan-suo-bfs-by-ywrx-y6lu/" xr:uid="{479482D9-B268-4348-9013-D7B5073218A6}"/>
+    <hyperlink ref="A19" r:id="rId17" display="https://leetcode.cn/problems/open-the-lock/solution/752-da-kai-zhuan-pan-suo-bfs-by-ywrx-y6lu/" xr:uid="{479482D9-B268-4348-9013-D7B5073218A6}"/>
     <hyperlink ref="A32" r:id="rId18" display="https://leetcode.cn/problems/serialize-and-deserialize-n-ary-tree/solution/-by-wywy-m-3tc6/" xr:uid="{8BE83A5B-40AC-A543-935A-56732443F452}"/>
     <hyperlink ref="A33" display="329 矩阵中的最长递增路径" xr:uid="{328B0723-66CE-B245-91ED-6BD40D9C8C2D}"/>
     <hyperlink ref="A24" r:id="rId19" display="https://leetcode.cn/problems/lexicographical-numbers/solution/by-wywy-m-zkeq/" xr:uid="{28DEC326-6FFF-FE45-9D81-FA88F9380338}"/>
@@ -4222,12 +4252,13 @@
     <hyperlink ref="A31" r:id="rId26" display="https://leetcode.cn/problems/number-of-distinct-islands/solution/-by-wywy-m-mnp1/" xr:uid="{466941BD-CCDE-314E-A33B-DDE50A357DDB}"/>
     <hyperlink ref="A34" r:id="rId27" display="https://leetcode.cn/problems/cracking-the-safe/solution/753-po-jie-bao-xian-xiang-tu-by-ywrx-sp9h/" xr:uid="{E7988CED-D4A4-354A-8874-C47FC910E55A}"/>
     <hyperlink ref="A35" r:id="rId28" xr:uid="{BC741E33-D794-4148-9FE5-2D8C789A48D5}"/>
+    <hyperlink ref="A21" r:id="rId29" xr:uid="{F7F1BE06-524D-3F45-A6A1-43D1A4059E77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F10A632-C78C-6347-8E5A-4720E264DA34}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -4514,7 +4545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB0168C-78E6-194A-941B-C4F6EE34E1A2}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -4772,6 +4803,215 @@
     <hyperlink ref="A20" r:id="rId17" display="https://leetcode.cn/problems/perfect-rectangle/solution/391-wan-mei-ju-xing-shu-xue-by-ywrx-nzcb/" xr:uid="{694FE087-F0FA-5544-BA9E-34B2B5115D74}"/>
     <hyperlink ref="A16" r:id="rId18" display="https://leetcode.cn/problems/get-kth-magic-number-lcci/solution/mian-shi-ti-1709-di-k-ge-shu-shu-xue-by-i0rvw/" xr:uid="{60A0FE99-59EB-9342-8EC9-C499A6B7D103}"/>
     <hyperlink ref="A17" r:id="rId19" display="https://leetcode.cn/problems/minimum-moves-to-equal-array-elements/solution/453-zui-xiao-cao-zuo-ci-shu-shi-shu-zu-y-jux0/" xr:uid="{7D95EC14-5D0E-2241-B657-124C5B842D1A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7589A38-5576-3242-8FA0-5F40561FA4C2}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20230227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20230227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>190</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>461</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20230307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20230227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>342</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>693</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>476</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>371</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>20211128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>20220620</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>137</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>260</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>338</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>318</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>20230311</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
+    <sortCondition ref="B2:B18" customList="E,M,H"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://leetcode.cn/problems/single-number/solution/136-zhi-chu-xian-yi-ci-de-shu-zi-bit-by-aysss/" xr:uid="{6838D459-36E5-C44B-BFDE-C5635CA20824}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://leetcode.cn/problems/number-of-1-bits/solution/191-wei-1de-ge-shu-by-ywrx-r1f3/" xr:uid="{9DDC3AB9-19E1-E04D-A0CB-5E28295BA66F}"/>
+    <hyperlink ref="A6" r:id="rId3" display="https://leetcode.cn/problems/missing-number/solution/268-diu-shi-de-shu-zi-bit-by-ywrx-si0w/" xr:uid="{FF558E44-4191-CB4D-8751-3009379D1378}"/>
+    <hyperlink ref="A7" r:id="rId4" display="https://leetcode.cn/problems/power-of-two/solution/231-2de-mi-bit-by-ywrx-irdd/" xr:uid="{A2EA1759-7E96-C348-A4C4-14CD318FEB9D}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://leetcode-cn.com/problems/add-binary/solution/67-er-jin-zhi-qiu-he-er-jin-zhi-by-wywy-xjbur/" xr:uid="{425415C8-27C2-7145-BA85-27F3506280BD}"/>
+    <hyperlink ref="A13" r:id="rId6" display="https://leetcode.cn/problems/is-unique-lcci/solution/pan-ding-zi-fu-shi-fou-wei-yi-bit-by-ywr-3rks/" xr:uid="{7D2F2735-0C48-B247-BFC8-1105E3BC7758}"/>
+    <hyperlink ref="A18" r:id="rId7" display="https://leetcode.cn/problems/cinema-seat-allocation/solution/1386-an-pai-dian-ying-yuan-zuo-wei-bit-b-l08z/" xr:uid="{577E6685-B9DD-754A-8E42-A51972308DDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5109,215 +5349,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7589A38-5576-3242-8FA0-5F40561FA4C2}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2">
-        <v>20230227</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>20230227</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>190</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>461</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>20230307</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2">
-        <v>20230227</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>342</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>693</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>476</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>371</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2">
-        <v>20211128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2">
-        <v>20220620</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>137</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>260</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>338</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>318</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2">
-        <v>20230311</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
-    <sortCondition ref="B2:B18" customList="E,M,H"/>
-  </sortState>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://leetcode.cn/problems/single-number/solution/136-zhi-chu-xian-yi-ci-de-shu-zi-bit-by-aysss/" xr:uid="{6838D459-36E5-C44B-BFDE-C5635CA20824}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://leetcode.cn/problems/number-of-1-bits/solution/191-wei-1de-ge-shu-by-ywrx-r1f3/" xr:uid="{9DDC3AB9-19E1-E04D-A0CB-5E28295BA66F}"/>
-    <hyperlink ref="A6" r:id="rId3" display="https://leetcode.cn/problems/missing-number/solution/268-diu-shi-de-shu-zi-bit-by-ywrx-si0w/" xr:uid="{FF558E44-4191-CB4D-8751-3009379D1378}"/>
-    <hyperlink ref="A7" r:id="rId4" display="https://leetcode.cn/problems/power-of-two/solution/231-2de-mi-bit-by-ywrx-irdd/" xr:uid="{A2EA1759-7E96-C348-A4C4-14CD318FEB9D}"/>
-    <hyperlink ref="A12" r:id="rId5" display="https://leetcode-cn.com/problems/add-binary/solution/67-er-jin-zhi-qiu-he-er-jin-zhi-by-wywy-xjbur/" xr:uid="{425415C8-27C2-7145-BA85-27F3506280BD}"/>
-    <hyperlink ref="A13" r:id="rId6" display="https://leetcode.cn/problems/is-unique-lcci/solution/pan-ding-zi-fu-shi-fou-wei-yi-bit-by-ywr-3rks/" xr:uid="{7D2F2735-0C48-B247-BFC8-1105E3BC7758}"/>
-    <hyperlink ref="A18" r:id="rId7" display="https://leetcode.cn/problems/cinema-seat-allocation/solution/1386-an-pai-dian-ying-yuan-zuo-wei-bit-b-l08z/" xr:uid="{577E6685-B9DD-754A-8E42-A51972308DDA}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB69C234-EDE8-3643-8B34-F99DBD5F82C4}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -5412,11 +5443,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF43907A-09FF-DA4F-B1FC-56FBDF277DF3}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -5427,123 +5458,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15">
         <v>20221020</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="16">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15">
         <v>20230317</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="16">
+      <c r="B4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="15">
         <v>20220911</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="16">
+      <c r="B5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15">
         <v>20220911</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="16">
+      <c r="B6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15">
         <v>20220913</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="16">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15">
         <v>20220914</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="16">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15">
         <v>20220918</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="16">
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15">
         <v>20221207</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="16">
+      <c r="B10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15">
         <v>20230309</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>347</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="16">
+      <c r="B11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15">
         <v>20230322</v>
       </c>
     </row>
@@ -5567,7 +5598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B14B54-A49B-D04E-8B69-DCDF1E44241B}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -5577,130 +5608,130 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="15"/>
-    <col min="3" max="3" width="14.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="52.6640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="14"/>
+    <col min="3" max="3" width="14.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15">
         <v>20220908</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="16">
+      <c r="B3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="15">
         <v>20220907</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="16">
+      <c r="B4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="15">
         <v>20220908</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="16">
+      <c r="B5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15">
         <v>20220911</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="16">
+      <c r="B6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15">
         <v>20220911</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="16">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15">
         <v>20230318</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="16">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15">
         <v>20230212</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>20220913</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>20230212</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>20230323</v>
       </c>
     </row>
@@ -5724,7 +5755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F89BF6-4A8D-664D-8E62-AB0D738DFAF1}">
   <dimension ref="A1:P7"/>
   <sheetViews>
@@ -5821,7 +5852,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>328</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5841,7 +5872,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>179</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -5858,7 +5889,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>123</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -5872,7 +5903,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5889,7 +5920,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>341</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -5952,7 +5983,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -5963,7 +5994,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5974,7 +6005,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -5985,7 +6016,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>340</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -6016,13 +6047,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.83203125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="12"/>
-    <col min="3" max="3" width="14.6640625" style="12" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="12"/>
+    <col min="1" max="1" width="49.83203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="11"/>
+    <col min="3" max="3" width="14.6640625" style="11" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -6819,10 +6850,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.33203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="10" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="10"/>
+    <col min="1" max="1" width="61.33203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6881,7 +6912,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -6892,7 +6923,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -6903,7 +6934,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -6914,7 +6945,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -6925,7 +6956,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -6936,7 +6967,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -6947,7 +6978,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -6958,7 +6989,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -6969,7 +7000,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -6980,7 +7011,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -6991,7 +7022,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -7002,7 +7033,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -7013,7 +7044,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -7024,7 +7055,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -7035,7 +7066,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -7046,7 +7077,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -7057,7 +7088,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -7068,7 +7099,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -7079,7 +7110,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -7090,7 +7121,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -7101,7 +7132,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>336</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -7411,10 +7442,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.83203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="10"/>
-    <col min="3" max="3" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="10"/>
+    <col min="1" max="1" width="61.83203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="9"/>
+    <col min="3" max="3" width="11.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7495,7 +7526,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>113</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -7506,7 +7537,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>114</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -7517,7 +7548,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -7539,7 +7570,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -7550,7 +7581,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -7561,7 +7592,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -7572,7 +7603,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>338</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -7583,7 +7614,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>337</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -7621,86 +7652,86 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="15"/>
-    <col min="3" max="3" width="14.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="15"/>
+    <col min="1" max="1" width="52.33203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="14"/>
+    <col min="3" max="3" width="14.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="16">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15">
         <v>20230110</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="16">
+      <c r="B3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="15">
         <v>20230323</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="16">
+      <c r="B4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="15">
         <v>20230109</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>20220620</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>20230110</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>20230316</v>
       </c>
     </row>

</xml_diff>

<commit_message>
03/27/23: Leetcode & ML Glossary
</commit_message>
<xml_diff>
--- a/Algorithms/Leetcode/Leetcode Catalog - Yu Wang.xlsx
+++ b/Algorithms/Leetcode/Leetcode Catalog - Yu Wang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuwang/Desktop/Notes/Algorithms/Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D824F3B-A021-394E-8B07-350F96CEE9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7AB41F-39C7-324D-A0C8-E54D1C77EA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="500" windowWidth="28040" windowHeight="15920" firstSheet="9" activeTab="15" xr2:uid="{D74CB876-27C2-064D-BD73-4428B59FF732}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="28040" windowHeight="15920" firstSheet="7" activeTab="8" xr2:uid="{D74CB876-27C2-064D-BD73-4428B59FF732}"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="5" r:id="rId1"/>
@@ -26,16 +26,15 @@
     <sheet name="Divide &amp; Conquer" sheetId="11" r:id="rId11"/>
     <sheet name="DP" sheetId="12" r:id="rId12"/>
     <sheet name="Greedy" sheetId="13" r:id="rId13"/>
-    <sheet name="Sheet2" sheetId="25" r:id="rId14"/>
-    <sheet name="Two Pointers" sheetId="14" r:id="rId15"/>
-    <sheet name="Graph" sheetId="15" r:id="rId16"/>
-    <sheet name="Backtrack" sheetId="16" r:id="rId17"/>
-    <sheet name="Math" sheetId="17" r:id="rId18"/>
-    <sheet name="Bit" sheetId="18" r:id="rId19"/>
-    <sheet name="Sliding Window" sheetId="19" r:id="rId20"/>
-    <sheet name="Simulation" sheetId="20" r:id="rId21"/>
-    <sheet name="OOD" sheetId="21" r:id="rId22"/>
-    <sheet name="Combined" sheetId="23" r:id="rId23"/>
+    <sheet name="Two Pointers" sheetId="14" r:id="rId14"/>
+    <sheet name="Graph" sheetId="15" r:id="rId15"/>
+    <sheet name="Backtrack" sheetId="16" r:id="rId16"/>
+    <sheet name="Math" sheetId="17" r:id="rId17"/>
+    <sheet name="Bit" sheetId="18" r:id="rId18"/>
+    <sheet name="Sliding Window" sheetId="19" r:id="rId19"/>
+    <sheet name="Simulation" sheetId="20" r:id="rId20"/>
+    <sheet name="OOD" sheetId="21" r:id="rId21"/>
+    <sheet name="Combined" sheetId="23" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="360">
   <si>
     <t>#</t>
   </si>
@@ -1106,6 +1105,36 @@
   </si>
   <si>
     <t>1293 网格中的最短路径</t>
+  </si>
+  <si>
+    <t>366 寻找二叉树的叶子结点</t>
+  </si>
+  <si>
+    <t>2034 股票价格波动</t>
+  </si>
+  <si>
+    <t>359 日志速率限制器</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>843 猜猜这个单词</t>
+  </si>
+  <si>
+    <t>2013 检测正方形</t>
+  </si>
+  <si>
+    <t>1937 扣分后的最大得分</t>
+  </si>
+  <si>
+    <t>2018 判断单词是否能放入填字游戏内</t>
+  </si>
+  <si>
+    <t>2178 拆分成最多数目的正偶数之和</t>
+  </si>
+  <si>
+    <t>729 我的日程安排表</t>
   </si>
 </sst>
 </file>
@@ -1323,15 +1352,13 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2008,236 +2035,236 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87904762-BFEC-434E-9C53-A84DD8444479}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="A19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
         <v>69</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
         <v>744</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
         <v>278</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="B4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
         <v>704</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
         <v>35</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15">
         <v>20221221</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
         <v>540</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15">
         <v>20221228</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15">
         <v>20220823</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
         <v>74</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="B10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
         <v>33</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="B11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="15">
         <v>81</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15">
         <v>20220823</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15">
         <v>20220925</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15">
         <v>20220927</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15">
         <v>20221219</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15">
         <v>20221220</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
         <v>154</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="C18" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="C20" s="15">
         <v>20220911</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15">
+        <v>20230327</v>
       </c>
     </row>
   </sheetData>
@@ -2248,13 +2275,13 @@
     <hyperlink ref="A8" r:id="rId1" display="https://leetcode-cn.com/problems/find-minimum-in-rotated-sorted-array/solution/153-xun-zhao-xuan-zhuan-pai-xu-shu-zu-zh-mjkr/" xr:uid="{97C09881-DE85-2B4C-B24D-348592E7CADD}"/>
     <hyperlink ref="A9" r:id="rId2" display="https://leetcode.cn/problems/find-first-and-last-position-of-element-in-sorted-array/solution/by-wywy-m-brqf/" xr:uid="{F885C336-C7F0-F340-B8B7-CDDAB9EDFAFA}"/>
     <hyperlink ref="A6" r:id="rId3" display="https://leetcode.cn/problems/search-insert-position/solution/35-by-wywy-m-upza/" xr:uid="{1BC04EE0-72B5-1849-ABC0-0DD006726EE2}"/>
-    <hyperlink ref="A19" r:id="rId4" display="https://leetcode-cn.com/problems/sliding-window-median/solution/480-hua-dong-chuang-kou-zhong-wei-shu-er-p3wx/" xr:uid="{962402DE-6ABF-E646-A2BD-A663C8AEFA25}"/>
-    <hyperlink ref="A13" r:id="rId5" display="https://leetcode.cn/problems/capacity-to-ship-packages-within-d-days/solution/by-wywy-m-9h37/" xr:uid="{7DFC3645-7076-B449-B401-7A66BFC435D5}"/>
-    <hyperlink ref="A20" r:id="rId6" display="https://leetcode.cn/problems/number-of-ships-in-a-rectangle/solution/-by-wywy-m-cpzm/" xr:uid="{6D6D6573-2537-0946-B1F1-76DDC4C7E142}"/>
-    <hyperlink ref="A14" r:id="rId7" display="https://leetcode.cn/problems/find-peak-element/solution/162-by-wywy-m-ca3f/" xr:uid="{A49B9F11-F12D-8348-98A9-1EAEACC53A17}"/>
-    <hyperlink ref="A15" r:id="rId8" display="https://leetcode.cn/problems/random-pick-with-weight/solution/by-wywy-m-otok/" xr:uid="{D52C6791-5ACF-4D45-B991-476C93EEDE33}"/>
-    <hyperlink ref="A16" r:id="rId9" display="https://leetcode.cn/problems/koko-eating-bananas/solution/-by-wywy-m-rgk4/" xr:uid="{2F79CBF3-CB9F-864B-9FA3-38F48A500C74}"/>
-    <hyperlink ref="A17" r:id="rId10" display="https://leetcode.cn/problems/peak-index-in-a-mountain-array/solution/-by-wywy-m-t5nn/" xr:uid="{F4141991-EED2-FD48-AA1B-BDDE998DEF52}"/>
+    <hyperlink ref="A13" r:id="rId4" display="https://leetcode.cn/problems/capacity-to-ship-packages-within-d-days/solution/by-wywy-m-9h37/" xr:uid="{7DFC3645-7076-B449-B401-7A66BFC435D5}"/>
+    <hyperlink ref="A20" r:id="rId5" display="https://leetcode.cn/problems/number-of-ships-in-a-rectangle/solution/-by-wywy-m-cpzm/" xr:uid="{6D6D6573-2537-0946-B1F1-76DDC4C7E142}"/>
+    <hyperlink ref="A14" r:id="rId6" display="https://leetcode.cn/problems/find-peak-element/solution/162-by-wywy-m-ca3f/" xr:uid="{A49B9F11-F12D-8348-98A9-1EAEACC53A17}"/>
+    <hyperlink ref="A15" r:id="rId7" display="https://leetcode.cn/problems/random-pick-with-weight/solution/by-wywy-m-otok/" xr:uid="{D52C6791-5ACF-4D45-B991-476C93EEDE33}"/>
+    <hyperlink ref="A16" r:id="rId8" display="https://leetcode.cn/problems/koko-eating-bananas/solution/-by-wywy-m-rgk4/" xr:uid="{2F79CBF3-CB9F-864B-9FA3-38F48A500C74}"/>
+    <hyperlink ref="A17" r:id="rId9" display="https://leetcode.cn/problems/peak-index-in-a-mountain-array/solution/-by-wywy-m-t5nn/" xr:uid="{F4141991-EED2-FD48-AA1B-BDDE998DEF52}"/>
+    <hyperlink ref="A21" r:id="rId10" xr:uid="{75D8F9F4-19F7-E547-8B84-32E6DC195CCE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2387,18 +2414,18 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF52CBDF-A54F-B64B-ABC7-BC9DA66EFACF}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.6640625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="19" style="22" customWidth="1"/>
-    <col min="3" max="3" width="29.5" style="22" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="22"/>
+    <col min="1" max="1" width="53.6640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="19" style="21" customWidth="1"/>
+    <col min="3" max="3" width="29.5" style="21" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -2985,7 +3012,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="16" t="s">
         <v>341</v>
       </c>
       <c r="B54" s="15" t="s">
@@ -2996,7 +3023,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="16" t="s">
         <v>348</v>
       </c>
       <c r="B55" s="18" t="s">
@@ -3004,6 +3031,17 @@
       </c>
       <c r="C55" s="18">
         <v>20230324</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="18">
+        <v>20230326</v>
       </c>
     </row>
   </sheetData>
@@ -3053,6 +3091,7 @@
     <hyperlink ref="A53" r:id="rId40" display="https://leetcode.cn/problems/maximum-number-of-books-you-can-take/solution/2355-ni-neng-na-zou-de-zui-da-tu-shu-shu-4cwe/" xr:uid="{CFA00C0F-A1B9-2143-9567-C1D46DE839B4}"/>
     <hyperlink ref="A54" r:id="rId41" xr:uid="{143774B1-1CB5-584A-A7EA-EFB7FAE785C2}"/>
     <hyperlink ref="A55" r:id="rId42" xr:uid="{9CE5EBF7-DFF5-8C4C-800C-035221F3521C}"/>
+    <hyperlink ref="A56" r:id="rId43" xr:uid="{2EEACA1F-B9C2-F445-AAC2-8786A0BEB3E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3060,10 +3099,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E45454-ABB5-A740-839B-4BC8D58C720C}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A1:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3446,6 +3485,17 @@
       </c>
       <c r="C34" s="15">
         <v>20230323</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A35" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="15">
+        <v>20230327</v>
       </c>
     </row>
   </sheetData>
@@ -3478,24 +3528,13 @@
     <hyperlink ref="A32" r:id="rId23" xr:uid="{E830922D-631C-A841-A908-BE96CF32A7D9}"/>
     <hyperlink ref="A33" r:id="rId24" xr:uid="{1BB1A7DC-260F-5547-A272-B29B3C31BC6A}"/>
     <hyperlink ref="A34" r:id="rId25" xr:uid="{C5B8642E-3DE7-F146-81F2-3585047BA96A}"/>
+    <hyperlink ref="A35" r:id="rId26" xr:uid="{215CC94D-85D2-5645-8285-6148AA47DB95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793BCECD-8B46-DA42-B72E-66FE64C4766E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F31A8D-9C09-434F-A40A-68C34FD0E968}">
   <dimension ref="A1:C27"/>
   <sheetViews>
@@ -3819,11 +3858,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3390D82-F280-2841-A652-0961C2865E3C}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -4070,7 +4109,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="22" t="s">
         <v>237</v>
       </c>
       <c r="B23" s="18"/>
@@ -4258,7 +4297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F10A632-C78C-6347-8E5A-4720E264DA34}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -4545,238 +4584,256 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB0168C-78E6-194A-941B-C4F6EE34E1A2}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.33203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="14"/>
+    <col min="3" max="3" width="14.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15">
         <v>20221129</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15">
         <v>20220925</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15">
         <v>20221219</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15">
         <v>20230225</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15">
         <v>20221129</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15">
         <v>20221219</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>272</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15">
         <v>20220912</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15">
         <v>20221010</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15">
         <v>20221213</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15">
         <v>20221220</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15">
         <v>20230225</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15">
         <v>20230225</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15">
         <v>20230226</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15">
         <v>20230226</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15">
         <v>20230308</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15">
         <v>20230312</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="15">
         <v>20220726</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="15">
         <v>20220913</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="15">
         <v>20230227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="15">
+        <v>20230326</v>
       </c>
     </row>
   </sheetData>
@@ -4803,12 +4860,13 @@
     <hyperlink ref="A20" r:id="rId17" display="https://leetcode.cn/problems/perfect-rectangle/solution/391-wan-mei-ju-xing-shu-xue-by-ywrx-nzcb/" xr:uid="{694FE087-F0FA-5544-BA9E-34B2B5115D74}"/>
     <hyperlink ref="A16" r:id="rId18" display="https://leetcode.cn/problems/get-kth-magic-number-lcci/solution/mian-shi-ti-1709-di-k-ge-shu-shu-xue-by-i0rvw/" xr:uid="{60A0FE99-59EB-9342-8EC9-C499A6B7D103}"/>
     <hyperlink ref="A17" r:id="rId19" display="https://leetcode.cn/problems/minimum-moves-to-equal-array-elements/solution/453-zui-xiao-cao-zuo-ci-shu-shi-shu-zu-y-jux0/" xr:uid="{7D95EC14-5D0E-2241-B657-124C5B842D1A}"/>
+    <hyperlink ref="A23" r:id="rId20" xr:uid="{C4A1BF58-7EB0-E04E-A4D3-133088260C64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7589A38-5576-3242-8FA0-5F40561FA4C2}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -5012,6 +5070,101 @@
     <hyperlink ref="A12" r:id="rId5" display="https://leetcode-cn.com/problems/add-binary/solution/67-er-jin-zhi-qiu-he-er-jin-zhi-by-wywy-xjbur/" xr:uid="{425415C8-27C2-7145-BA85-27F3506280BD}"/>
     <hyperlink ref="A13" r:id="rId6" display="https://leetcode.cn/problems/is-unique-lcci/solution/pan-ding-zi-fu-shi-fou-wei-yi-bit-by-ywr-3rks/" xr:uid="{7D2F2735-0C48-B247-BFC8-1105E3BC7758}"/>
     <hyperlink ref="A18" r:id="rId7" display="https://leetcode.cn/problems/cinema-seat-allocation/solution/1386-an-pai-dian-ying-yuan-zuo-wei-bit-b-l08z/" xr:uid="{577E6685-B9DD-754A-8E42-A51972308DDA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB69C234-EDE8-3643-8B34-F99DBD5F82C4}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20220823</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20220823</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20220823</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20220925</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20220823</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C6">
+    <sortCondition ref="B2:B6" customList="E,M,H"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" display="https://leetcode.cn/problems/minimum-window-substring/solution/-by-wywy-m-4hkf/" xr:uid="{586C3D79-F444-EE44-AE54-56E600B621B0}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://leetcode.cn/problems/permutation-in-string/solution/567-zi-fu-chuan-de-pai-lie-by-wywy-m-q1ts/" xr:uid="{2517D657-6FDF-2C42-B7E5-78624A2E7708}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://leetcode.cn/problems/find-all-anagrams-in-a-string/submissions/" xr:uid="{EBF4977C-672D-CA4A-A9C6-B64D0B827A2F}"/>
+    <hyperlink ref="A4" r:id="rId4" display="https://leetcode.cn/problems/longest-substring-without-repeating-characters/solution/3-wu-zhong-fu-zi-fu-chuan-de-zui-chang-z-fkie/" xr:uid="{D10DC5BA-2CF7-7C43-A026-3D3D46E2FF79}"/>
+    <hyperlink ref="A5" r:id="rId5" display="https://leetcode.cn/problems/longest-repeating-character-replacement/solution/424-ti-huan-hou-de-zui-chang-zhong-fu-zi-djg2/" xr:uid="{F2FA77A7-AA80-3243-B2BC-2B7820F310A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5349,111 +5502,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB69C234-EDE8-3643-8B34-F99DBD5F82C4}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF43907A-09FF-DA4F-B1FC-56FBDF277DF3}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2">
-        <v>20220823</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>20220823</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>20220823</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>20220925</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>20220823</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C6">
-    <sortCondition ref="B2:B6" customList="E,M,H"/>
-  </sortState>
-  <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="https://leetcode.cn/problems/minimum-window-substring/solution/-by-wywy-m-4hkf/" xr:uid="{586C3D79-F444-EE44-AE54-56E600B621B0}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://leetcode.cn/problems/permutation-in-string/solution/567-zi-fu-chuan-de-pai-lie-by-wywy-m-q1ts/" xr:uid="{2517D657-6FDF-2C42-B7E5-78624A2E7708}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://leetcode.cn/problems/find-all-anagrams-in-a-string/submissions/" xr:uid="{EBF4977C-672D-CA4A-A9C6-B64D0B827A2F}"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://leetcode.cn/problems/longest-substring-without-repeating-characters/solution/3-wu-zhong-fu-zi-fu-chuan-de-zui-chang-z-fkie/" xr:uid="{D10DC5BA-2CF7-7C43-A026-3D3D46E2FF79}"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://leetcode.cn/problems/longest-repeating-character-replacement/solution/424-ti-huan-hou-de-zui-chang-zhong-fu-zi-djg2/" xr:uid="{F2FA77A7-AA80-3243-B2BC-2B7820F310A2}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF43907A-09FF-DA4F-B1FC-56FBDF277DF3}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="46.5" customWidth="1"/>
+    <col min="1" max="1" width="58.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5576,6 +5634,17 @@
       </c>
       <c r="C11" s="15">
         <v>20230322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15">
+        <v>20230327</v>
       </c>
     </row>
   </sheetData>
@@ -5593,12 +5662,13 @@
     <hyperlink ref="A10" r:id="rId8" display="https://leetcode.cn/problems/find-missing-observations/solution/2028-zhao-chu-que-shi-de-guan-ce-shu-ju-wagg4/" xr:uid="{1345FCC1-8DF4-7B4D-856A-79217DE8026F}"/>
     <hyperlink ref="A3" r:id="rId9" display="https://leetcode.cn/problems/find-n-unique-integers-sum-up-to-zero/solution/1304-he-wei-ling-de-n-ge-bu-tong-zheng-s-oi7x/" xr:uid="{E5523D15-7AF9-B043-A0B1-6976D5C2D31D}"/>
     <hyperlink ref="A11" r:id="rId10" xr:uid="{19B31EC3-C3AB-A540-AA50-BC43CAFAAB4E}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{8FD603C7-23F2-7B4E-A68C-A318C10DFFAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B14B54-A49B-D04E-8B69-DCDF1E44241B}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -5755,7 +5825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F89BF6-4A8D-664D-8E62-AB0D738DFAF1}">
   <dimension ref="A1:P7"/>
   <sheetViews>
@@ -5780,37 +5850,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="24" t="s">
         <v>326</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24" t="s">
         <v>325</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4" t="s">
         <v>334</v>
       </c>
@@ -6039,502 +6109,513 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A9675C-39F8-DD4C-B84E-2CBC8BF054BB}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.83203125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="65.6640625" style="11" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="11"/>
     <col min="3" max="3" width="14.6640625" style="11" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" s="12" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15">
         <v>20230213</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
         <v>543</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
         <v>226</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="B4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
         <v>617</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
         <v>112</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
         <v>572</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
         <v>101</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="15">
         <v>20230220</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
         <v>404</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="B10" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
         <v>687</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="B11" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="15">
         <v>671</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="B12" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A13" s="15">
         <v>637</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="15">
         <v>20230213</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="15">
         <v>20230213</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="15">
         <v>20230213</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15">
         <v>20230214</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15">
         <v>20230314</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
         <v>337</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="B19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
         <v>513</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
         <v>144</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="B21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
         <v>94</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B22" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="B23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="15">
         <v>20220814</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="B24" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="15">
         <v>20220824</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B25" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="15">
         <v>20220824</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B26" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="15">
         <v>20220824</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2">
+      <c r="B27" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="15">
         <v>20220824</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B28" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="15">
         <v>20220824</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B29" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="15">
         <v>20220905</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="B30" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="15">
         <v>20220913</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2">
+      <c r="B31" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="15">
         <v>20220926</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="2">
+      <c r="B32" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="15">
         <v>20220927</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="2">
+      <c r="B33" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="15">
         <v>20230213</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="2">
+      <c r="B34" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="15">
         <v>20230214</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2">
+      <c r="B35" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="15">
         <v>20230214</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2">
+      <c r="B36" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="15">
         <v>20230319</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
         <v>318</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="2">
+      <c r="B37" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="15">
         <v>20230319</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+    <row r="38" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A38" s="15">
         <v>145</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="C38" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A39" s="15">
         <v>1028</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="C39" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="15">
         <v>20220927</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A41" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="15">
         <v>20220913</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A42" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="15">
         <v>20220925</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A43" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="15">
         <v>20230214</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A44" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="4">
+      <c r="B44" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="18">
         <v>20230322</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A45" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="18">
+        <v>20230325</v>
       </c>
     </row>
   </sheetData>
@@ -6569,6 +6650,7 @@
     <hyperlink ref="A36" r:id="rId25" xr:uid="{AA8650A6-4615-7A48-AF6E-58593930E8BC}"/>
     <hyperlink ref="A37" r:id="rId26" xr:uid="{7EFDD8E6-A5D9-D243-BF9C-174B93993794}"/>
     <hyperlink ref="A44" r:id="rId27" xr:uid="{CC14A0A8-50CC-D847-829E-993E8EF49BDF}"/>
+    <hyperlink ref="A45" r:id="rId28" xr:uid="{3524C6A1-4A90-054F-AC10-D37588A6DB15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6842,304 +6924,326 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C38DCB7-D208-4A47-A52C-374E9CD57FFC}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="75.33203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="9" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" style="9" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
         <v>217</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
         <v>594</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="B4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
         <v>242</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15">
         <v>20220626</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15">
         <v>20220917</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="B8" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15">
         <v>12.18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15">
         <v>12.27</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15">
         <v>20220623</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15">
         <v>20220911</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="15">
         <v>20220913</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15">
         <v>20220918</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="15">
         <v>20220918</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15">
         <v>20220927</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="15">
         <v>20221010</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15">
         <v>20230312</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="15">
         <v>20230314</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15">
         <v>20230316</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15">
         <v>20230318</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="15">
         <v>20220919</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="15">
         <v>20220920</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="15">
         <v>20230212</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="15">
         <v>20230212</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="26" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="B26" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="15">
         <v>20230321</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="14">
+        <v>20230325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="14">
+        <v>20230326</v>
       </c>
     </row>
   </sheetData>
@@ -7168,6 +7272,8 @@
     <hyperlink ref="A20" r:id="rId19" display="https://leetcode.cn/problems/minimum-number-of-keypresses/solution/2268-zui-shao-an-jian-ci-shu-hashmap-by-dowte/" xr:uid="{8ABFAC54-A220-2641-90E7-B808D0CA0F1E}"/>
     <hyperlink ref="A21" r:id="rId20" display="https://leetcode.cn/problems/maximal-network-rank/solution/1615-zui-da-wang-luo-zhi-hash-by-ywrx-xbkk/" xr:uid="{0222E21B-5E2A-A749-805E-180C098BF0E8}"/>
     <hyperlink ref="A26" r:id="rId21" xr:uid="{B1E177DD-FD5A-4348-965A-48AFFA38F669}"/>
+    <hyperlink ref="A27" r:id="rId22" xr:uid="{9FAECA00-4CB3-5E4C-8E05-9C17ECD83DDF}"/>
+    <hyperlink ref="A28" r:id="rId23" xr:uid="{30A2B5A7-1793-D846-9A1F-B579B41E0CEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7644,10 +7750,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA87E2-0C96-3045-BD9E-C5C85205F434}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -7735,6 +7841,28 @@
         <v>20230316</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="14">
+        <v>20230325</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="15">
+        <v>20230327</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C7">
     <sortCondition ref="B2:B7" customList="E,M,H"/>
@@ -7746,6 +7874,8 @@
     <hyperlink ref="A2" r:id="rId4" display="https://leetcode.cn/problems/kth-largest-element-in-a-stream/solution/703-shu-ju-liu-zhong-de-di-by-wywy-m-nxnu/" xr:uid="{1E7C1BB8-783E-5041-ADA7-51127C3F71E7}"/>
     <hyperlink ref="A6" r:id="rId5" display="https://leetcode.cn/problems/find-median-from-data-stream/solution/-by-wywy-m-1paq/" xr:uid="{D3579325-3524-7843-BDB0-9D2510D1A33C}"/>
     <hyperlink ref="A7" r:id="rId6" display="https://leetcode.cn/problems/maximum-number-of-robots-within-budget/solution/2398-yu-suan-nei-de-zui-duo-ji-qi-ren-sh-c2r7/" xr:uid="{3E7F95E0-F88B-8B4E-BB5A-48442AB5849A}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{CFD18935-3DE1-7247-9859-1F5FFA29B74F}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://leetcode-cn.com/problems/sliding-window-median/solution/480-hua-dong-chuang-kou-zhong-wei-shu-er-p3wx/" xr:uid="{962402DE-6ABF-E646-A2BD-A663C8AEFA25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
04/02/23: Leetcode, Vim, Shell and Git
</commit_message>
<xml_diff>
--- a/Algorithms/Leetcode/Leetcode Catalog - Yu Wang.xlsx
+++ b/Algorithms/Leetcode/Leetcode Catalog - Yu Wang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuwang/Desktop/Notes/Algorithms/Leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7AB41F-39C7-324D-A0C8-E54D1C77EA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB2B7F4-CBB5-FC43-B3B2-6DA226D6F145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28040" windowHeight="15920" firstSheet="7" activeTab="8" xr2:uid="{D74CB876-27C2-064D-BD73-4428B59FF732}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15920" firstSheet="4" activeTab="5" xr2:uid="{D74CB876-27C2-064D-BD73-4428B59FF732}"/>
   </bookViews>
   <sheets>
     <sheet name="Array" sheetId="5" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="367">
   <si>
     <t>#</t>
   </si>
@@ -1135,6 +1135,27 @@
   </si>
   <si>
     <t>729 我的日程安排表</t>
+  </si>
+  <si>
+    <t>1048 最长字符串链</t>
+  </si>
+  <si>
+    <t>2115 从给定原材料中找出所有可以做出的菜</t>
+  </si>
+  <si>
+    <t>715 range模块</t>
+  </si>
+  <si>
+    <t>1101 彼此熟识的最早时间</t>
+  </si>
+  <si>
+    <t>562 矩阵中最长的连续1线段</t>
+  </si>
+  <si>
+    <t>1055 形成字符串的最短路径</t>
+  </si>
+  <si>
+    <t>1146 快照数组</t>
   </si>
 </sst>
 </file>
@@ -2037,17 +2058,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87904762-BFEC-434E-9C53-A84DD8444479}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="A19:C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="77.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.33203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="14"/>
+    <col min="3" max="3" width="14.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2058,7 +2081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15">
         <v>69</v>
       </c>
@@ -2069,7 +2092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>744</v>
       </c>
@@ -2080,7 +2103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>278</v>
       </c>
@@ -2091,7 +2114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>704</v>
       </c>
@@ -2102,7 +2125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>35</v>
       </c>
@@ -2113,7 +2136,7 @@
         <v>20221221</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>540</v>
       </c>
@@ -2124,7 +2147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>124</v>
       </c>
@@ -2135,7 +2158,7 @@
         <v>20221228</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>125</v>
       </c>
@@ -2146,7 +2169,7 @@
         <v>20220823</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>74</v>
       </c>
@@ -2157,7 +2180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>33</v>
       </c>
@@ -2168,7 +2191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <v>81</v>
       </c>
@@ -2179,7 +2202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>127</v>
       </c>
@@ -2190,7 +2213,7 @@
         <v>20220823</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>129</v>
       </c>
@@ -2201,7 +2224,7 @@
         <v>20220925</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>130</v>
       </c>
@@ -2209,10 +2232,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="15">
-        <v>20220927</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+        <v>20230330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>131</v>
       </c>
@@ -2223,7 +2246,7 @@
         <v>20221219</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>132</v>
       </c>
@@ -2234,7 +2257,7 @@
         <v>20221220</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>154</v>
       </c>
@@ -2245,43 +2268,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
         <v>128</v>
       </c>
+      <c r="B19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="15">
+        <v>20220911</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>359</v>
+      </c>
       <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15">
+        <v>20230327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="15">
-        <v>20220911</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>359</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>5</v>
-      </c>
       <c r="C21" s="15">
-        <v>20230327</v>
+        <v>20230328</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C20">
-    <sortCondition ref="B2:B20" customList="E,M,H"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C19">
+    <sortCondition ref="B2:B19" customList="E,M,H"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="A8" r:id="rId1" display="https://leetcode-cn.com/problems/find-minimum-in-rotated-sorted-array/solution/153-xun-zhao-xuan-zhuan-pai-xu-shu-zu-zh-mjkr/" xr:uid="{97C09881-DE85-2B4C-B24D-348592E7CADD}"/>
     <hyperlink ref="A9" r:id="rId2" display="https://leetcode.cn/problems/find-first-and-last-position-of-element-in-sorted-array/solution/by-wywy-m-brqf/" xr:uid="{F885C336-C7F0-F340-B8B7-CDDAB9EDFAFA}"/>
     <hyperlink ref="A6" r:id="rId3" display="https://leetcode.cn/problems/search-insert-position/solution/35-by-wywy-m-upza/" xr:uid="{1BC04EE0-72B5-1849-ABC0-0DD006726EE2}"/>
     <hyperlink ref="A13" r:id="rId4" display="https://leetcode.cn/problems/capacity-to-ship-packages-within-d-days/solution/by-wywy-m-9h37/" xr:uid="{7DFC3645-7076-B449-B401-7A66BFC435D5}"/>
-    <hyperlink ref="A20" r:id="rId5" display="https://leetcode.cn/problems/number-of-ships-in-a-rectangle/solution/-by-wywy-m-cpzm/" xr:uid="{6D6D6573-2537-0946-B1F1-76DDC4C7E142}"/>
+    <hyperlink ref="A19" r:id="rId5" display="https://leetcode.cn/problems/number-of-ships-in-a-rectangle/solution/-by-wywy-m-cpzm/" xr:uid="{6D6D6573-2537-0946-B1F1-76DDC4C7E142}"/>
     <hyperlink ref="A14" r:id="rId6" display="https://leetcode.cn/problems/find-peak-element/solution/162-by-wywy-m-ca3f/" xr:uid="{A49B9F11-F12D-8348-98A9-1EAEACC53A17}"/>
-    <hyperlink ref="A15" r:id="rId7" display="https://leetcode.cn/problems/random-pick-with-weight/solution/by-wywy-m-otok/" xr:uid="{D52C6791-5ACF-4D45-B991-476C93EEDE33}"/>
+    <hyperlink ref="A15" r:id="rId7" xr:uid="{D52C6791-5ACF-4D45-B991-476C93EEDE33}"/>
     <hyperlink ref="A16" r:id="rId8" display="https://leetcode.cn/problems/koko-eating-bananas/solution/-by-wywy-m-rgk4/" xr:uid="{2F79CBF3-CB9F-864B-9FA3-38F48A500C74}"/>
     <hyperlink ref="A17" r:id="rId9" display="https://leetcode.cn/problems/peak-index-in-a-mountain-array/solution/-by-wywy-m-t5nn/" xr:uid="{F4141991-EED2-FD48-AA1B-BDDE998DEF52}"/>
-    <hyperlink ref="A21" r:id="rId10" xr:uid="{75D8F9F4-19F7-E547-8B84-32E6DC195CCE}"/>
+    <hyperlink ref="A20" r:id="rId10" xr:uid="{75D8F9F4-19F7-E547-8B84-32E6DC195CCE}"/>
+    <hyperlink ref="A21" r:id="rId11" xr:uid="{B6228B73-C7EF-C847-B5B7-AAE94E9E74E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2414,10 +2449,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF52CBDF-A54F-B64B-ABC7-BC9DA66EFACF}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -3042,6 +3077,28 @@
       </c>
       <c r="C56" s="18">
         <v>20230326</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="18">
+        <v>20230328</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="18">
+        <v>20230330</v>
       </c>
     </row>
   </sheetData>
@@ -3092,6 +3149,8 @@
     <hyperlink ref="A54" r:id="rId41" xr:uid="{143774B1-1CB5-584A-A7EA-EFB7FAE785C2}"/>
     <hyperlink ref="A55" r:id="rId42" xr:uid="{9CE5EBF7-DFF5-8C4C-800C-035221F3521C}"/>
     <hyperlink ref="A56" r:id="rId43" xr:uid="{2EEACA1F-B9C2-F445-AAC2-8786A0BEB3E0}"/>
+    <hyperlink ref="A57" r:id="rId44" xr:uid="{286CC1FD-7E03-5749-92A5-A0A9607D8F81}"/>
+    <hyperlink ref="A58" r:id="rId45" xr:uid="{044A2DB8-AE62-4444-8E98-6D605D3D8BC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3860,15 +3919,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3390D82-F280-2841-A652-0961C2865E3C}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="70.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="4"/>
     <col min="3" max="3" width="14.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="4"/>
@@ -3970,198 +4029,198 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="A10" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15">
+        <v>20230328</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>226</v>
+        <v>363</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="15">
-        <v>1</v>
+        <v>20230329</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="15">
-        <v>1</v>
-      </c>
+      <c r="A12" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="15">
-        <v>20220612</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>229</v>
+      <c r="A14" s="15" t="s">
+        <v>227</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="15">
-        <v>20220912</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="15">
-        <v>20220914</v>
+        <v>20220612</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="15">
-        <v>20220917</v>
+        <v>20220912</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="15">
-        <v>20220926</v>
+        <v>20220914</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="15">
-        <v>20221020</v>
+        <v>20220917</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="15">
-        <v>20230220</v>
+        <v>20220926</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C20" s="15">
-        <v>20221018</v>
+        <v>20221020</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>349</v>
+        <v>236</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C21" s="15">
-        <v>20230324</v>
+        <v>20230220</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="15">
-        <v>20230220</v>
+        <v>20221018</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="15">
+        <v>20230324</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C24" s="15">
-        <v>20220925</v>
+        <v>20230220</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="15">
-        <v>20230219</v>
-      </c>
+      <c r="A25" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
     </row>
     <row r="26" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="15">
-        <v>20220906</v>
+        <v>20220925</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="15">
-        <v>20220906</v>
+        <v>20230219</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>5</v>
@@ -4172,7 +4231,7 @@
     </row>
     <row r="29" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>5</v>
@@ -4183,7 +4242,7 @@
     </row>
     <row r="30" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>5</v>
@@ -4194,7 +4253,7 @@
     </row>
     <row r="31" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>5</v>
@@ -4205,61 +4264,83 @@
     </row>
     <row r="32" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C32" s="15">
-        <v>20220913</v>
+        <v>20220906</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C33" s="15">
-        <v>20220923</v>
+        <v>20220906</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="15">
-        <v>20230308</v>
+        <v>20220913</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="26" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
-        <v>317</v>
+        <v>239</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="15">
+        <v>20220923</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="15">
+        <v>20230308</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="15">
         <v>20230319</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:C22">
-    <sortCondition ref="B11:B22" customList="E,M,H"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:C24">
+    <sortCondition ref="B13:B24" customList="E,M,H"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="https://leetcode.cn/problems/all-paths-from-source-to-target/solution/by-wywy-m-nqp0/" xr:uid="{62AA1BDA-9AEF-1D4E-985F-E4BFC300F9ED}"/>
@@ -4269,29 +4350,31 @@
     <hyperlink ref="A7" r:id="rId5" display="https://leetcode.cn/problems/course-schedule-ii/solution/210-ke-cheng-biao-iigraph-by-wywy-m-18nk/" xr:uid="{C7EEFC8F-2387-F14A-B36C-A22ACD69ECCB}"/>
     <hyperlink ref="A8" r:id="rId6" display="https://leetcode.cn/problems/network-delay-time/solution/743-wang-luo-yan-chi-shi-jian-dijkstra-b-6zyo/" xr:uid="{FC2F7E70-70B6-EC40-83E9-F14EEDE1A2B2}"/>
     <hyperlink ref="A9" r:id="rId7" display="https://leetcode.cn/problems/min-cost-to-connect-all-points/solution/1584-lian-jie-suo-you-dian-de-zui-xiao-f-dtmy/" xr:uid="{D6E252E8-6A56-B449-917D-D9191B43E8F1}"/>
-    <hyperlink ref="A11" r:id="rId8" display="https://leetcode-cn.com/problems/shortest-path-in-binary-matrix/solution/1091-er-jin-zhi-ju-zhen-zui-duan-lu-jing-00dr/" xr:uid="{678CC0D2-5BB2-9447-A9D9-85A1922DAD7A}"/>
-    <hyperlink ref="A13" r:id="rId9" display="https://leetcode.cn/problems/ji-qi-ren-de-yun-dong-fan-wei-lcof/solution/-by-wywy-m-hks2/" xr:uid="{433B27C5-3ADF-6344-8B10-3C6FE890D909}"/>
-    <hyperlink ref="A14" r:id="rId10" display="https://leetcode.cn/problems/web-crawler/solution/by-wywy-m-tq5x/" xr:uid="{1096138D-EBE2-324D-A769-E0CF4843CC45}"/>
-    <hyperlink ref="A15" r:id="rId11" display="https://leetcode.cn/problems/populating-next-right-pointers-in-each-node-ii/solution/117-by-wywy-m-2dey/" xr:uid="{DB4092D2-CEB5-5F40-9A2F-A3D1F3E1FAD5}"/>
-    <hyperlink ref="A16" r:id="rId12" display="https://leetcode.cn/problems/evaluate-division/solution/by-wywy-m-fqcc/" xr:uid="{3BA99F54-D69C-BE40-BD52-19CC44580857}"/>
-    <hyperlink ref="A17" r:id="rId13" display="https://leetcode.cn/problems/walls-and-gates/solution/286-by-wywy-m-v89r/" xr:uid="{A1807D7E-F45A-BC4D-A674-450FE3CC3465}"/>
-    <hyperlink ref="A20" r:id="rId14" display="https://leetcode.cn/problems/shortest-distance-from-all-buildings/solution/317-by-wywy-m-31q4/" xr:uid="{7C3F06B2-F6CE-D941-A3E6-9CC13D48726B}"/>
-    <hyperlink ref="A18" r:id="rId15" display="https://leetcode.cn/problems/01-matrix/solution/-by-wywy-m-1ak4/" xr:uid="{AC1F76FF-A2DA-694F-A769-2136BC16C971}"/>
-    <hyperlink ref="A22" r:id="rId16" display="https://leetcode.cn/problems/sliding-puzzle/solution/773-hua-dong-mi-ti-bfs-by-ywrx-c74s/" xr:uid="{0AD32694-5038-3D45-918C-C400FC7946DE}"/>
-    <hyperlink ref="A19" r:id="rId17" display="https://leetcode.cn/problems/open-the-lock/solution/752-da-kai-zhuan-pan-suo-bfs-by-ywrx-y6lu/" xr:uid="{479482D9-B268-4348-9013-D7B5073218A6}"/>
-    <hyperlink ref="A32" r:id="rId18" display="https://leetcode.cn/problems/serialize-and-deserialize-n-ary-tree/solution/-by-wywy-m-3tc6/" xr:uid="{8BE83A5B-40AC-A543-935A-56732443F452}"/>
-    <hyperlink ref="A33" display="329 矩阵中的最长递增路径" xr:uid="{328B0723-66CE-B245-91ED-6BD40D9C8C2D}"/>
-    <hyperlink ref="A24" r:id="rId19" display="https://leetcode.cn/problems/lexicographical-numbers/solution/by-wywy-m-zkeq/" xr:uid="{28DEC326-6FFF-FE45-9D81-FA88F9380338}"/>
-    <hyperlink ref="A25" r:id="rId20" display="https://leetcode.cn/problems/surrounded-regions/solution/130-bei-wei-rao-de-qu-yu-dfs-by-ywrx-mgaq/" xr:uid="{8185D2DF-B947-7249-A9B8-CB74F896DE51}"/>
-    <hyperlink ref="A26" r:id="rId21" display="https://leetcode.cn/problems/number-of-islands/solution/200-dao-yu-shu-liang-by-wywy-m-cxtr/" xr:uid="{FF9132AC-9049-064B-B540-E8D27BD1C30B}"/>
-    <hyperlink ref="A27" r:id="rId22" display="https://leetcode.cn/problems/number-of-closed-islands/solution/1254-tong-ji-feng-bi-by-wywy-m-qc5d/" xr:uid="{7F2AB7CB-072B-9448-BB8B-4B7470CEC5CE}"/>
-    <hyperlink ref="A28" r:id="rId23" display="https://leetcode.cn/problems/number-of-enclaves/solution/1020-fei-di-by-wywy-m-n8fe/" xr:uid="{BACB5764-3CC5-A84C-8DC0-4FD405B3E874}"/>
-    <hyperlink ref="A29" r:id="rId24" display="https://leetcode.cn/problems/max-area-of-island/solution/695-by-wywy-m-iuv4/" xr:uid="{17FBEAD3-6BD2-B54B-AFE1-BCD179AE4565}"/>
-    <hyperlink ref="A30" r:id="rId25" display="https://leetcode.cn/problems/count-sub-islands/solution/1905-tong-ji-zi-dao-yu-by-wywy-m-txx9/" xr:uid="{93A063DA-39C1-0549-B8E6-6D257572601D}"/>
-    <hyperlink ref="A31" r:id="rId26" display="https://leetcode.cn/problems/number-of-distinct-islands/solution/-by-wywy-m-mnp1/" xr:uid="{466941BD-CCDE-314E-A33B-DDE50A357DDB}"/>
-    <hyperlink ref="A34" r:id="rId27" display="https://leetcode.cn/problems/cracking-the-safe/solution/753-po-jie-bao-xian-xiang-tu-by-ywrx-sp9h/" xr:uid="{E7988CED-D4A4-354A-8874-C47FC910E55A}"/>
-    <hyperlink ref="A35" r:id="rId28" xr:uid="{BC741E33-D794-4148-9FE5-2D8C789A48D5}"/>
-    <hyperlink ref="A21" r:id="rId29" xr:uid="{F7F1BE06-524D-3F45-A6A1-43D1A4059E77}"/>
+    <hyperlink ref="A13" r:id="rId8" display="https://leetcode-cn.com/problems/shortest-path-in-binary-matrix/solution/1091-er-jin-zhi-ju-zhen-zui-duan-lu-jing-00dr/" xr:uid="{678CC0D2-5BB2-9447-A9D9-85A1922DAD7A}"/>
+    <hyperlink ref="A15" r:id="rId9" display="https://leetcode.cn/problems/ji-qi-ren-de-yun-dong-fan-wei-lcof/solution/-by-wywy-m-hks2/" xr:uid="{433B27C5-3ADF-6344-8B10-3C6FE890D909}"/>
+    <hyperlink ref="A16" r:id="rId10" display="https://leetcode.cn/problems/web-crawler/solution/by-wywy-m-tq5x/" xr:uid="{1096138D-EBE2-324D-A769-E0CF4843CC45}"/>
+    <hyperlink ref="A17" r:id="rId11" display="https://leetcode.cn/problems/populating-next-right-pointers-in-each-node-ii/solution/117-by-wywy-m-2dey/" xr:uid="{DB4092D2-CEB5-5F40-9A2F-A3D1F3E1FAD5}"/>
+    <hyperlink ref="A18" r:id="rId12" display="https://leetcode.cn/problems/evaluate-division/solution/by-wywy-m-fqcc/" xr:uid="{3BA99F54-D69C-BE40-BD52-19CC44580857}"/>
+    <hyperlink ref="A19" r:id="rId13" display="https://leetcode.cn/problems/walls-and-gates/solution/286-by-wywy-m-v89r/" xr:uid="{A1807D7E-F45A-BC4D-A674-450FE3CC3465}"/>
+    <hyperlink ref="A22" r:id="rId14" display="https://leetcode.cn/problems/shortest-distance-from-all-buildings/solution/317-by-wywy-m-31q4/" xr:uid="{7C3F06B2-F6CE-D941-A3E6-9CC13D48726B}"/>
+    <hyperlink ref="A20" r:id="rId15" display="https://leetcode.cn/problems/01-matrix/solution/-by-wywy-m-1ak4/" xr:uid="{AC1F76FF-A2DA-694F-A769-2136BC16C971}"/>
+    <hyperlink ref="A24" r:id="rId16" display="https://leetcode.cn/problems/sliding-puzzle/solution/773-hua-dong-mi-ti-bfs-by-ywrx-c74s/" xr:uid="{0AD32694-5038-3D45-918C-C400FC7946DE}"/>
+    <hyperlink ref="A21" r:id="rId17" display="https://leetcode.cn/problems/open-the-lock/solution/752-da-kai-zhuan-pan-suo-bfs-by-ywrx-y6lu/" xr:uid="{479482D9-B268-4348-9013-D7B5073218A6}"/>
+    <hyperlink ref="A34" r:id="rId18" display="https://leetcode.cn/problems/serialize-and-deserialize-n-ary-tree/solution/-by-wywy-m-3tc6/" xr:uid="{8BE83A5B-40AC-A543-935A-56732443F452}"/>
+    <hyperlink ref="A35" display="329 矩阵中的最长递增路径" xr:uid="{328B0723-66CE-B245-91ED-6BD40D9C8C2D}"/>
+    <hyperlink ref="A26" r:id="rId19" display="https://leetcode.cn/problems/lexicographical-numbers/solution/by-wywy-m-zkeq/" xr:uid="{28DEC326-6FFF-FE45-9D81-FA88F9380338}"/>
+    <hyperlink ref="A27" r:id="rId20" display="https://leetcode.cn/problems/surrounded-regions/solution/130-bei-wei-rao-de-qu-yu-dfs-by-ywrx-mgaq/" xr:uid="{8185D2DF-B947-7249-A9B8-CB74F896DE51}"/>
+    <hyperlink ref="A28" r:id="rId21" display="https://leetcode.cn/problems/number-of-islands/solution/200-dao-yu-shu-liang-by-wywy-m-cxtr/" xr:uid="{FF9132AC-9049-064B-B540-E8D27BD1C30B}"/>
+    <hyperlink ref="A29" r:id="rId22" display="https://leetcode.cn/problems/number-of-closed-islands/solution/1254-tong-ji-feng-bi-by-wywy-m-qc5d/" xr:uid="{7F2AB7CB-072B-9448-BB8B-4B7470CEC5CE}"/>
+    <hyperlink ref="A30" r:id="rId23" display="https://leetcode.cn/problems/number-of-enclaves/solution/1020-fei-di-by-wywy-m-n8fe/" xr:uid="{BACB5764-3CC5-A84C-8DC0-4FD405B3E874}"/>
+    <hyperlink ref="A31" r:id="rId24" display="https://leetcode.cn/problems/max-area-of-island/solution/695-by-wywy-m-iuv4/" xr:uid="{17FBEAD3-6BD2-B54B-AFE1-BCD179AE4565}"/>
+    <hyperlink ref="A32" r:id="rId25" display="https://leetcode.cn/problems/count-sub-islands/solution/1905-tong-ji-zi-dao-yu-by-wywy-m-txx9/" xr:uid="{93A063DA-39C1-0549-B8E6-6D257572601D}"/>
+    <hyperlink ref="A33" r:id="rId26" display="https://leetcode.cn/problems/number-of-distinct-islands/solution/-by-wywy-m-mnp1/" xr:uid="{466941BD-CCDE-314E-A33B-DDE50A357DDB}"/>
+    <hyperlink ref="A36" r:id="rId27" display="https://leetcode.cn/problems/cracking-the-safe/solution/753-po-jie-bao-xian-xiang-tu-by-ywrx-sp9h/" xr:uid="{E7988CED-D4A4-354A-8874-C47FC910E55A}"/>
+    <hyperlink ref="A37" r:id="rId28" xr:uid="{BC741E33-D794-4148-9FE5-2D8C789A48D5}"/>
+    <hyperlink ref="A23" r:id="rId29" xr:uid="{F7F1BE06-524D-3F45-A6A1-43D1A4059E77}"/>
+    <hyperlink ref="A10" r:id="rId30" xr:uid="{0E22DCEF-0BC9-3444-97D4-2AB1C84A8351}"/>
+    <hyperlink ref="A11" r:id="rId31" xr:uid="{287B3E6D-9056-694F-B287-0EF92D0296AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4588,7 +4671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB0168C-78E6-194A-941B-C4F6EE34E1A2}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -6924,17 +7007,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C38DCB7-D208-4A47-A52C-374E9CD57FFC}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75.33203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="9" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
@@ -7214,7 +7297,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>336</v>
       </c>
       <c r="B26" s="15" t="s">
@@ -7225,25 +7308,47 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="16" t="s">
         <v>352</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="14">
+      <c r="B27" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="18">
         <v>20230325</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="26" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="16" t="s">
         <v>355</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="14">
+      <c r="B28" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="18">
         <v>20230326</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="18">
+        <v>20230401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="26" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="18">
+        <v>20230401</v>
       </c>
     </row>
   </sheetData>
@@ -7274,6 +7379,8 @@
     <hyperlink ref="A26" r:id="rId21" xr:uid="{B1E177DD-FD5A-4348-965A-48AFFA38F669}"/>
     <hyperlink ref="A27" r:id="rId22" xr:uid="{9FAECA00-4CB3-5E4C-8E05-9C17ECD83DDF}"/>
     <hyperlink ref="A28" r:id="rId23" xr:uid="{30A2B5A7-1793-D846-9A1F-B579B41E0CEF}"/>
+    <hyperlink ref="A29" r:id="rId24" xr:uid="{209BED91-FED1-E344-83AE-DBA906F973B8}"/>
+    <hyperlink ref="A30" r:id="rId25" xr:uid="{A7409944-9E1F-4543-B4B4-9D8AF255C01E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7752,7 +7859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA87E2-0C96-3045-BD9E-C5C85205F434}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>